<commit_message>
hay que arreglar el bug de procesamiento de eventos y el rnd de servidor
</commit_message>
<xml_diff>
--- a/simulacion_peluqueria.xlsx
+++ b/simulacion_peluqueria.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
   <si>
     <t>nro_fila</t>
   </si>
@@ -181,33 +181,33 @@
     <t>Llegada cliente 3</t>
   </si>
   <si>
+    <t>Llegada cliente 4</t>
+  </si>
+  <si>
+    <t>Fin servicio Peluquero A</t>
+  </si>
+  <si>
     <t>Fin servicio Peluquero B</t>
   </si>
   <si>
-    <t>Llegada cliente 4</t>
-  </si>
-  <si>
     <t>Llegada cliente 5</t>
   </si>
   <si>
     <t>Llegada cliente 6</t>
   </si>
   <si>
-    <t>Paga refrigerio 3</t>
-  </si>
-  <si>
     <t>Llegada cliente 7</t>
   </si>
   <si>
     <t>Peluquero B</t>
   </si>
   <si>
+    <t>Peluquero A</t>
+  </si>
+  <si>
     <t>Colorista</t>
   </si>
   <si>
-    <t>Peluquero A</t>
-  </si>
-  <si>
     <t>Libre</t>
   </si>
   <si>
@@ -217,19 +217,22 @@
     <t>SAPB</t>
   </si>
   <si>
+    <t>SAPA</t>
+  </si>
+  <si>
+    <t>EAPA (50.1)</t>
+  </si>
+  <si>
+    <t>EAPB (59.3)</t>
+  </si>
+  <si>
     <t>SAC</t>
   </si>
   <si>
-    <t>EAC (60.4)</t>
-  </si>
-  <si>
-    <t>EAC (68.59)</t>
-  </si>
-  <si>
-    <t>SAPA</t>
-  </si>
-  <si>
-    <t>EAPA (92.9)</t>
+    <t>EAPB (71.4)</t>
+  </si>
+  <si>
+    <t>EAC (80.3)</t>
   </si>
 </sst>
 </file>
@@ -726,16 +729,16 @@
         <v>51</v>
       </c>
       <c r="E2">
-        <v>0.96</v>
+        <v>0.44</v>
       </c>
       <c r="F2">
-        <v>11.6</v>
+        <v>6.4</v>
       </c>
       <c r="G2">
-        <v>11.6</v>
+        <v>6.4</v>
       </c>
       <c r="H2">
-        <v>0.89</v>
+        <v>0.62</v>
       </c>
       <c r="I2" t="s">
         <v>61</v>
@@ -791,7 +794,7 @@
         <v>41</v>
       </c>
       <c r="B3">
-        <v>11.6</v>
+        <v>6.4</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
@@ -800,16 +803,16 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.55</v>
+        <v>0.11</v>
       </c>
       <c r="F3">
-        <v>7.5</v>
+        <v>3.1</v>
       </c>
       <c r="G3">
-        <v>19.1</v>
+        <v>9.5</v>
       </c>
       <c r="H3">
-        <v>0.89</v>
+        <v>0.62</v>
       </c>
       <c r="I3" t="s">
         <v>61</v>
@@ -827,13 +830,13 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0.06</v>
+        <v>0.54</v>
       </c>
       <c r="R3">
-        <v>22.96</v>
+        <v>30.64</v>
       </c>
       <c r="S3">
-        <v>34.56</v>
+        <v>37.04</v>
       </c>
       <c r="T3" t="s">
         <v>65</v>
@@ -877,7 +880,7 @@
         <v>42</v>
       </c>
       <c r="B4">
-        <v>19.1</v>
+        <v>9.5</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
@@ -886,13 +889,13 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>0.93</v>
+        <v>0.86</v>
       </c>
       <c r="F4">
-        <v>11.3</v>
+        <v>10.6</v>
       </c>
       <c r="G4">
-        <v>30.4</v>
+        <v>20.1</v>
       </c>
       <c r="I4" t="s">
         <v>62</v>
@@ -903,32 +906,32 @@
       <c r="K4" t="b">
         <v>0</v>
       </c>
+      <c r="L4">
+        <v>0.31</v>
+      </c>
+      <c r="M4">
+        <v>22.24</v>
+      </c>
+      <c r="N4">
+        <v>31.74</v>
+      </c>
       <c r="O4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>37.04</v>
+      </c>
+      <c r="T4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
         <v>64</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>34.56</v>
-      </c>
-      <c r="T4" t="s">
-        <v>65</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0.72</v>
-      </c>
-      <c r="W4">
-        <v>44.4</v>
-      </c>
-      <c r="X4">
-        <v>63.5</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>65</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -966,7 +969,7 @@
         <v>43</v>
       </c>
       <c r="B5">
-        <v>30.4</v>
+        <v>20.1</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
@@ -975,13 +978,13 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0.62</v>
+        <v>0.72</v>
       </c>
       <c r="F5">
-        <v>8.19</v>
+        <v>9.19</v>
       </c>
       <c r="G5">
-        <v>38.6</v>
+        <v>29.3</v>
       </c>
       <c r="I5" t="s">
         <v>62</v>
@@ -992,29 +995,29 @@
       <c r="K5" t="b">
         <v>0</v>
       </c>
+      <c r="N5">
+        <v>31.74</v>
+      </c>
       <c r="O5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>37.04</v>
+      </c>
+      <c r="T5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
         <v>64</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>34.56</v>
-      </c>
-      <c r="T5" t="s">
-        <v>65</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>63.5</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>65</v>
-      </c>
       <c r="Z5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -1052,16 +1055,25 @@
         <v>44</v>
       </c>
       <c r="B6">
-        <v>34.56</v>
+        <v>29.3</v>
       </c>
       <c r="C6" t="s">
         <v>55</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>0.6</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>38.6</v>
+        <v>37.29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>61</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -1069,56 +1081,62 @@
       <c r="K6" t="b">
         <v>0</v>
       </c>
+      <c r="N6">
+        <v>31.74</v>
+      </c>
       <c r="O6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>37.04</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="s">
         <v>64</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>34.56</v>
-      </c>
-      <c r="T6" t="s">
-        <v>64</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>63.5</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>65</v>
-      </c>
       <c r="Z6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>18000</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>18000</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <v>1</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG6" t="b">
         <v>0</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>66</v>
       </c>
       <c r="AI6" t="s">
         <v>67</v>
       </c>
       <c r="AJ6" t="s">
         <v>68</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:40">
@@ -1126,25 +1144,16 @@
         <v>45</v>
       </c>
       <c r="B7">
-        <v>38.6</v>
+        <v>31.74</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
       </c>
       <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>0.66</v>
-      </c>
-      <c r="F7">
-        <v>8.6</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>47.2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>62</v>
+        <v>37.29</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -1152,26 +1161,35 @@
       <c r="K7" t="b">
         <v>0</v>
       </c>
+      <c r="L7">
+        <v>0.38</v>
+      </c>
+      <c r="M7">
+        <v>22.52</v>
+      </c>
+      <c r="N7">
+        <v>54.26</v>
+      </c>
       <c r="O7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>37.04</v>
+      </c>
+      <c r="T7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="s">
         <v>64</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="T7" t="s">
-        <v>64</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>63.5</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>65</v>
-      </c>
       <c r="Z7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA7">
         <v>18000</v>
@@ -1186,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="AE7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <v>2</v>
@@ -1194,11 +1212,11 @@
       <c r="AG7" t="b">
         <v>0</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AH7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>67</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>68</v>
       </c>
       <c r="AK7" t="s">
         <v>69</v>
@@ -1209,25 +1227,16 @@
         <v>46</v>
       </c>
       <c r="B8">
-        <v>47.2</v>
+        <v>37.04</v>
       </c>
       <c r="C8" t="s">
         <v>57</v>
       </c>
       <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>0.27</v>
-      </c>
-      <c r="F8">
-        <v>4.7</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>51.9</v>
-      </c>
-      <c r="I8" t="s">
-        <v>63</v>
+        <v>37.29</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -1235,14 +1244,8 @@
       <c r="K8" t="b">
         <v>0</v>
       </c>
-      <c r="L8">
-        <v>0.03</v>
-      </c>
-      <c r="M8">
-        <v>21.12</v>
-      </c>
       <c r="N8">
-        <v>68.31999999999999</v>
+        <v>54.26</v>
       </c>
       <c r="O8" t="s">
         <v>65</v>
@@ -1250,35 +1253,41 @@
       <c r="P8">
         <v>0</v>
       </c>
+      <c r="Q8">
+        <v>0.6</v>
+      </c>
+      <c r="R8">
+        <v>31.6</v>
+      </c>
+      <c r="S8">
+        <v>68.64</v>
+      </c>
       <c r="T8" t="s">
+        <v>65</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
         <v>64</v>
       </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>63.5</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>65</v>
-      </c>
       <c r="Z8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>18000</v>
+        <v>36000</v>
       </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>18000</v>
+        <v>36000</v>
       </c>
       <c r="AD8">
         <v>1</v>
       </c>
       <c r="AE8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF8">
         <v>2</v>
@@ -1286,17 +1295,11 @@
       <c r="AG8" t="b">
         <v>0</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AJ8" t="s">
         <v>67</v>
       </c>
-      <c r="AJ8" t="s">
-        <v>68</v>
-      </c>
       <c r="AK8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:40">
@@ -1304,25 +1307,25 @@
         <v>47</v>
       </c>
       <c r="B9">
-        <v>51.9</v>
+        <v>37.29</v>
       </c>
       <c r="C9" t="s">
         <v>58</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>0.9</v>
+        <v>0.21</v>
       </c>
       <c r="F9">
-        <v>11</v>
+        <v>4.09</v>
       </c>
       <c r="G9">
-        <v>62.9</v>
+        <v>41.4</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -1331,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>68.31999999999999</v>
+        <v>54.26</v>
       </c>
       <c r="O9" t="s">
         <v>65</v>
@@ -1339,14 +1342,8 @@
       <c r="P9">
         <v>0</v>
       </c>
-      <c r="Q9">
-        <v>0.35</v>
-      </c>
-      <c r="R9">
-        <v>27.6</v>
-      </c>
       <c r="S9">
-        <v>79.5</v>
+        <v>68.64</v>
       </c>
       <c r="T9" t="s">
         <v>65</v>
@@ -1354,29 +1351,35 @@
       <c r="U9">
         <v>0</v>
       </c>
+      <c r="V9">
+        <v>0.43</v>
+      </c>
+      <c r="W9">
+        <v>38.6</v>
+      </c>
       <c r="X9">
-        <v>63.5</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="Y9" t="s">
         <v>65</v>
       </c>
       <c r="Z9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA9">
-        <v>18000</v>
+        <v>36000</v>
       </c>
       <c r="AB9">
         <v>0</v>
       </c>
       <c r="AC9">
-        <v>18000</v>
+        <v>36000</v>
       </c>
       <c r="AD9">
         <v>1</v>
       </c>
       <c r="AE9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF9">
         <v>2</v>
@@ -1384,20 +1387,14 @@
       <c r="AG9" t="b">
         <v>0</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AJ9" t="s">
         <v>67</v>
       </c>
-      <c r="AJ9" t="s">
-        <v>68</v>
-      </c>
       <c r="AK9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AL9" t="s">
         <v>70</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:40">
@@ -1405,16 +1402,25 @@
         <v>48</v>
       </c>
       <c r="B10">
-        <v>60.4</v>
+        <v>41.4</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F10">
+        <v>8.890000000000001</v>
       </c>
       <c r="G10">
-        <v>62.9</v>
+        <v>50.3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -1423,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>68.31999999999999</v>
+        <v>54.26</v>
       </c>
       <c r="O10" t="s">
         <v>65</v>
@@ -1432,37 +1438,37 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>79.5</v>
+        <v>68.64</v>
       </c>
       <c r="T10" t="s">
         <v>65</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <v>63.5</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="Y10" t="s">
         <v>65</v>
       </c>
       <c r="Z10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA10">
-        <v>18000</v>
+        <v>36000</v>
       </c>
       <c r="AB10">
-        <v>6500</v>
+        <v>0</v>
       </c>
       <c r="AC10">
-        <v>11500</v>
+        <v>36000</v>
       </c>
       <c r="AD10">
         <v>1</v>
       </c>
       <c r="AE10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF10">
         <v>2</v>
@@ -1470,20 +1476,17 @@
       <c r="AG10" t="b">
         <v>0</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AJ10" t="s">
         <v>67</v>
       </c>
-      <c r="AJ10" t="s">
-        <v>68</v>
-      </c>
       <c r="AK10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AL10" t="s">
         <v>70</v>
       </c>
       <c r="AM10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:40">
@@ -1491,7 +1494,7 @@
         <v>49</v>
       </c>
       <c r="B11">
-        <v>62.9</v>
+        <v>50.3</v>
       </c>
       <c r="C11" t="s">
         <v>60</v>
@@ -1500,13 +1503,13 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>0.99</v>
+        <v>0.77</v>
       </c>
       <c r="F11">
-        <v>11.9</v>
+        <v>9.69</v>
       </c>
       <c r="G11">
-        <v>74.8</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
         <v>63</v>
@@ -1518,70 +1521,67 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>68.31999999999999</v>
+        <v>54.26</v>
       </c>
       <c r="O11" t="s">
         <v>65</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>79.5</v>
+        <v>68.64</v>
       </c>
       <c r="T11" t="s">
         <v>65</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <v>63.5</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="Y11" t="s">
         <v>65</v>
       </c>
       <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>36000</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>36000</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11">
         <v>2</v>
       </c>
-      <c r="AA11">
-        <v>18000</v>
-      </c>
-      <c r="AB11">
-        <v>6500</v>
-      </c>
-      <c r="AC11">
-        <v>11500</v>
-      </c>
-      <c r="AD11">
-        <v>1</v>
-      </c>
-      <c r="AE11">
-        <v>3</v>
-      </c>
       <c r="AF11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG11" t="b">
         <v>0</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AJ11" t="s">
         <v>67</v>
       </c>
-      <c r="AJ11" t="s">
-        <v>68</v>
-      </c>
       <c r="AK11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AL11" t="s">
         <v>70</v>
       </c>
       <c r="AM11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="AN11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:40">
@@ -1589,13 +1589,13 @@
         <v>50</v>
       </c>
       <c r="B12">
-        <v>842.46</v>
+        <v>883.92</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D12">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -1610,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>842.46</v>
+        <v>883.92</v>
       </c>
       <c r="T12" t="s">
         <v>64</v>
@@ -1625,13 +1625,13 @@
         <v>0</v>
       </c>
       <c r="AA12">
-        <v>1443000</v>
+        <v>1516000</v>
       </c>
       <c r="AB12">
         <v>344500</v>
       </c>
       <c r="AC12">
-        <v>1098500</v>
+        <v>1171500</v>
       </c>
       <c r="AD12">
         <v>1</v>
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="AF12">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AG12" t="b">
         <v>1</v>

</xml_diff>